<commit_message>
Update RL results figure
</commit_message>
<xml_diff>
--- a/benchmarks/rl-hyper-params.xlsx
+++ b/benchmarks/rl-hyper-params.xlsx
@@ -101,12 +101,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="H32" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Aaron Snoswell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Needs to be 0.0?</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="91">
   <si>
     <t>Parameter</t>
   </si>
@@ -379,16 +403,13 @@
   </si>
   <si>
     <t>Ours</t>
-  </si>
-  <si>
-    <t>256, 32</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,6 +437,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -629,7 +663,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -679,6 +712,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -963,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -972,91 +1008,91 @@
     <col min="1" max="1" width="27.3046875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.61328125" style="13" customWidth="1"/>
     <col min="3" max="3" width="12" style="8" customWidth="1"/>
-    <col min="4" max="4" width="11.53515625" style="3" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="11.53515625" style="8" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="13.15234375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="14.69140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.53515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.53515625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="13.15234375" style="8" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14.69140625" style="8" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="14.69140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="6"/>
       <c r="B1" s="12"/>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="22"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="7"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="31" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="35" t="s">
+      <c r="E2" s="31"/>
+      <c r="F2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="32"/>
-      <c r="H2" s="22"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="33" t="s">
+      <c r="C3" s="28"/>
+      <c r="D3" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="26" t="s">
+      <c r="E3" s="26"/>
+      <c r="F3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="27"/>
+      <c r="G3" s="26"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="34" t="s">
+      <c r="C4" s="28"/>
+      <c r="D4" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="28" t="s">
+      <c r="E4" s="28"/>
+      <c r="F4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="29"/>
+      <c r="G4" s="28"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="34" t="s">
+      <c r="C5" s="28"/>
+      <c r="D5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="29"/>
-      <c r="F5" s="28" t="s">
+      <c r="E5" s="28"/>
+      <c r="F5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="29"/>
+      <c r="G5" s="28"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
@@ -1080,7 +1116,7 @@
       <c r="G7" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="21" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1115,7 +1151,7 @@
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-      <c r="H9" s="24"/>
+      <c r="H9" s="23"/>
       <c r="I9" t="s">
         <v>58</v>
       </c>
@@ -1131,7 +1167,7 @@
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
-      <c r="H10" s="24"/>
+      <c r="H10" s="23"/>
       <c r="I10" t="s">
         <v>59</v>
       </c>
@@ -1147,7 +1183,7 @@
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
-      <c r="H11" s="24"/>
+      <c r="H11" s="23"/>
       <c r="I11" t="s">
         <v>60</v>
       </c>
@@ -1163,7 +1199,7 @@
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
-      <c r="H12" s="24"/>
+      <c r="H12" s="23"/>
       <c r="I12" t="s">
         <v>61</v>
       </c>
@@ -1182,7 +1218,7 @@
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
-      <c r="H13" s="24"/>
+      <c r="H13" s="23"/>
       <c r="I13" t="s">
         <v>62</v>
       </c>
@@ -1201,7 +1237,7 @@
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
-      <c r="H14" s="24"/>
+      <c r="H14" s="23"/>
       <c r="I14" t="s">
         <v>63</v>
       </c>
@@ -1217,7 +1253,7 @@
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="23"/>
       <c r="I15" t="s">
         <v>64</v>
       </c>
@@ -1233,7 +1269,7 @@
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="24"/>
+      <c r="H16" s="23"/>
       <c r="I16" t="s">
         <v>65</v>
       </c>
@@ -1252,7 +1288,7 @@
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="24"/>
+      <c r="H17" s="23"/>
       <c r="I17" t="s">
         <v>66</v>
       </c>
@@ -1268,7 +1304,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="24"/>
+      <c r="H18" s="23"/>
       <c r="I18" t="s">
         <v>67</v>
       </c>
@@ -1287,7 +1323,7 @@
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
-      <c r="H19" s="24"/>
+      <c r="H19" s="23"/>
       <c r="I19" t="s">
         <v>68</v>
       </c>
@@ -1306,7 +1342,7 @@
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
-      <c r="H20" s="24">
+      <c r="H20" s="23">
         <v>256</v>
       </c>
       <c r="I20" t="s">
@@ -1324,7 +1360,7 @@
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
-      <c r="H21" s="24"/>
+      <c r="H21" s="23"/>
       <c r="I21" t="s">
         <v>70</v>
       </c>
@@ -1340,7 +1376,7 @@
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
-      <c r="H22" s="24"/>
+      <c r="H22" s="23"/>
       <c r="I22" t="s">
         <v>71</v>
       </c>
@@ -1356,7 +1392,7 @@
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
-      <c r="H23" s="24"/>
+      <c r="H23" s="23"/>
       <c r="I23" t="s">
         <v>72</v>
       </c>
@@ -1372,7 +1408,7 @@
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
-      <c r="H24" s="25">
+      <c r="H24" s="24">
         <v>1E-4</v>
       </c>
       <c r="I24" t="s">
@@ -1390,7 +1426,7 @@
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
-      <c r="H25" s="25">
+      <c r="H25" s="24">
         <v>1E-4</v>
       </c>
       <c r="I25" t="s">
@@ -1408,7 +1444,7 @@
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
-      <c r="H26" s="24"/>
+      <c r="H26" s="23"/>
       <c r="I26" t="s">
         <v>75</v>
       </c>
@@ -1424,7 +1460,7 @@
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
-      <c r="H27" s="24"/>
+      <c r="H27" s="23"/>
       <c r="I27" t="s">
         <v>76</v>
       </c>
@@ -1461,16 +1497,16 @@
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
-      <c r="H29" s="24"/>
+      <c r="H29" s="23"/>
       <c r="I29" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="H30" s="24"/>
+      <c r="H30" s="23"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B31" s="15"/>
@@ -1487,15 +1523,15 @@
       <c r="G31" s="8">
         <v>5</v>
       </c>
-      <c r="H31" s="24" t="s">
-        <v>91</v>
+      <c r="H31" s="23">
+        <v>256</v>
       </c>
       <c r="I31" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B32" s="15"/>
@@ -1512,7 +1548,7 @@
       <c r="G32" s="8">
         <v>0.01</v>
       </c>
-      <c r="H32" s="24">
+      <c r="H32" s="35">
         <v>0.01</v>
       </c>
       <c r="I32" t="s">
@@ -1520,7 +1556,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B33" s="15"/>
@@ -1534,7 +1570,7 @@
       <c r="G33" s="8">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="H33" s="25">
+      <c r="H33" s="24">
         <v>1E-4</v>
       </c>
       <c r="I33" t="s">
@@ -1556,7 +1592,7 @@
       <c r="G34" s="8">
         <v>0.25</v>
       </c>
-      <c r="H34" s="24"/>
+      <c r="H34" s="23"/>
       <c r="I34" t="s">
         <v>29</v>
       </c>
@@ -1573,13 +1609,13 @@
       <c r="G35" s="8">
         <v>0.5</v>
       </c>
-      <c r="H35" s="24"/>
+      <c r="H35" s="23"/>
       <c r="I35" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="18" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A36" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B36" s="15"/>
@@ -1589,13 +1625,13 @@
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
-      <c r="H36" s="24"/>
+      <c r="H36" s="23"/>
       <c r="I36" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="18" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A37" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B37" s="15"/>
@@ -1608,13 +1644,13 @@
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
-      <c r="H37" s="24"/>
+      <c r="H37" s="23"/>
       <c r="I37" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="18" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A38" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B38" s="15"/>
@@ -1627,13 +1663,13 @@
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
-      <c r="H38" s="24"/>
+      <c r="H38" s="23"/>
       <c r="I38" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="18" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A39" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B39" s="15"/>
@@ -1643,13 +1679,12 @@
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
-      <c r="H39" s="24"/>
+      <c r="H39" s="23"/>
       <c r="I39" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.4"/>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
         <v>83</v>
       </c>
@@ -1657,7 +1692,7 @@
       <c r="C41" s="10"/>
       <c r="D41" s="17"/>
       <c r="E41" s="10"/>
-      <c r="F41" s="20"/>
+      <c r="F41" s="19"/>
       <c r="G41" s="8">
         <v>0.99</v>
       </c>
@@ -1665,7 +1700,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
         <v>84</v>
       </c>
@@ -1673,7 +1708,7 @@
       <c r="C42" s="10"/>
       <c r="D42" s="17"/>
       <c r="E42" s="10"/>
-      <c r="F42" s="20"/>
+      <c r="F42" s="19"/>
       <c r="G42" s="8">
         <v>5.0000000000000002E-5</v>
       </c>
@@ -1681,7 +1716,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
         <v>82</v>
       </c>
@@ -1689,13 +1724,13 @@
       <c r="C43" s="10"/>
       <c r="D43" s="17"/>
       <c r="E43" s="10"/>
-      <c r="F43" s="21" t="s">
+      <c r="F43" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="G43" s="19" t="s">
+      <c r="G43" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="H43" s="23" t="s">
+      <c r="H43" s="22" t="s">
         <v>89</v>
       </c>
       <c r="I43" t="s">

</xml_diff>